<commit_message>
Added distance matrix and driving time matrix using Bing API truck route
</commit_message>
<xml_diff>
--- a/Travel Matrix.xlsx
+++ b/Travel Matrix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Addresses" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Distance-Matrix" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Driving-Time-Matrix" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -22,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -35,6 +37,12 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF1A73E8"/>
+      <sz val="9"/>
     </font>
     <font>
       <b val="1"/>
@@ -90,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -105,7 +113,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -505,56 +514,56 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Node</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Fuel station Name</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Service</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Country Code</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Postal Code</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
@@ -651,7 +660,6 @@
           <t>Port Stanley</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>North Ward, Port Stanley, ON N5L 1B3</t>
@@ -714,11 +722,12 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>62.57421112</v>
+        <v>43.066721</v>
       </c>
       <c r="I5" t="n">
-        <v>-96.60791016</v>
-      </c>
+        <v>-80.797623</v>
+      </c>
+      <c r="J5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -837,11 +846,12 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>62.57421112</v>
+        <v>43.434777</v>
       </c>
       <c r="I8" t="n">
-        <v>-96.60791016</v>
-      </c>
+        <v>-80.24607399999999</v>
+      </c>
+      <c r="J8" s="6" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1057,7 +1067,6 @@
           <t>Detroit</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>Romulus, MI 48242, United States</t>
@@ -1092,7 +1101,6 @@
           <t>Windsor</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>3200 County Rd 42 Unit #200, Windsor, ON N8V 0A1</t>
@@ -1129,7 +1137,6 @@
           <t>Sarnia</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>125 Green St, Sarnia, ON N7T 2K4</t>
@@ -1166,7 +1173,6 @@
           <t>Barrie</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
           <t>41 Mapleview Dr E, Barrie, ON L4N 9A9</t>
@@ -1203,7 +1209,6 @@
           <t>Ottawa</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
           <t>1487 Merivale Rd, Nepean, ON K2E 5P3</t>
@@ -1240,7 +1245,6 @@
           <t>Montreal</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
           <t>Bd Roméo Vachon Nord (Arrivées), Dorval, QC H4Y 1H1</t>
@@ -1277,7 +1281,6 @@
           <t>Toronto</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>44 Cotswold Crescent, Toronto, ON M2P 1N2</t>
@@ -1314,7 +1317,6 @@
           <t>Cambridge</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
           <t>1055 Fountain St N, Cambridge, ON N3H 4R7</t>
@@ -1359,7 +1361,7 @@
       <selection activeCell="A1" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
@@ -1458,7 +1460,7 @@
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
@@ -3816,7 +3818,7 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -4664,7 +4666,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -4705,7 +4707,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="n">
@@ -4784,7 +4786,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
@@ -4816,4 +4818,2766 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="U1" s="7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>134.394</v>
+      </c>
+      <c r="E2" t="n">
+        <v>175.377</v>
+      </c>
+      <c r="F2" t="n">
+        <v>179.147</v>
+      </c>
+      <c r="G2" t="n">
+        <v>261.548</v>
+      </c>
+      <c r="H2" t="n">
+        <v>260.604</v>
+      </c>
+      <c r="I2" t="n">
+        <v>418.767</v>
+      </c>
+      <c r="J2" t="n">
+        <v>390.369</v>
+      </c>
+      <c r="K2" t="n">
+        <v>624.894</v>
+      </c>
+      <c r="L2" t="n">
+        <v>624.894</v>
+      </c>
+      <c r="M2" t="n">
+        <v>724.736</v>
+      </c>
+      <c r="N2" t="n">
+        <v>92.98999999999999</v>
+      </c>
+      <c r="O2" t="n">
+        <v>45.889</v>
+      </c>
+      <c r="P2" t="n">
+        <v>110.626</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>376.229</v>
+      </c>
+      <c r="R2" t="n">
+        <v>700.191</v>
+      </c>
+      <c r="S2" t="n">
+        <v>834.938</v>
+      </c>
+      <c r="T2" t="n">
+        <v>323.579</v>
+      </c>
+      <c r="U2" t="n">
+        <v>231.679</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>134.394</v>
+      </c>
+      <c r="E3" t="n">
+        <v>175.377</v>
+      </c>
+      <c r="F3" t="n">
+        <v>179.147</v>
+      </c>
+      <c r="G3" t="n">
+        <v>261.548</v>
+      </c>
+      <c r="H3" t="n">
+        <v>260.604</v>
+      </c>
+      <c r="I3" t="n">
+        <v>418.767</v>
+      </c>
+      <c r="J3" t="n">
+        <v>390.369</v>
+      </c>
+      <c r="K3" t="n">
+        <v>624.894</v>
+      </c>
+      <c r="L3" t="n">
+        <v>624.894</v>
+      </c>
+      <c r="M3" t="n">
+        <v>724.736</v>
+      </c>
+      <c r="N3" t="n">
+        <v>92.98999999999999</v>
+      </c>
+      <c r="O3" t="n">
+        <v>45.889</v>
+      </c>
+      <c r="P3" t="n">
+        <v>110.626</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>376.229</v>
+      </c>
+      <c r="R3" t="n">
+        <v>700.191</v>
+      </c>
+      <c r="S3" t="n">
+        <v>834.938</v>
+      </c>
+      <c r="T3" t="n">
+        <v>323.579</v>
+      </c>
+      <c r="U3" t="n">
+        <v>231.679</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>135.671</v>
+      </c>
+      <c r="C4" t="n">
+        <v>135.671</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>71.66800000000001</v>
+      </c>
+      <c r="F4" t="n">
+        <v>75.438</v>
+      </c>
+      <c r="G4" t="n">
+        <v>157.839</v>
+      </c>
+      <c r="H4" t="n">
+        <v>156.895</v>
+      </c>
+      <c r="I4" t="n">
+        <v>315.058</v>
+      </c>
+      <c r="J4" t="n">
+        <v>286.668</v>
+      </c>
+      <c r="K4" t="n">
+        <v>521.193</v>
+      </c>
+      <c r="L4" t="n">
+        <v>521.193</v>
+      </c>
+      <c r="M4" t="n">
+        <v>621.708</v>
+      </c>
+      <c r="N4" t="n">
+        <v>237.002</v>
+      </c>
+      <c r="O4" t="n">
+        <v>189.901</v>
+      </c>
+      <c r="P4" t="n">
+        <v>127.178</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>272.52</v>
+      </c>
+      <c r="R4" t="n">
+        <v>596.482</v>
+      </c>
+      <c r="S4" t="n">
+        <v>731.237</v>
+      </c>
+      <c r="T4" t="n">
+        <v>219.87</v>
+      </c>
+      <c r="U4" t="n">
+        <v>127.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>185.249</v>
+      </c>
+      <c r="C5" t="n">
+        <v>185.249</v>
+      </c>
+      <c r="D5" t="n">
+        <v>82.53400000000001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10.679</v>
+      </c>
+      <c r="G5" t="n">
+        <v>86.342</v>
+      </c>
+      <c r="H5" t="n">
+        <v>85.398</v>
+      </c>
+      <c r="I5" t="n">
+        <v>243.561</v>
+      </c>
+      <c r="J5" t="n">
+        <v>215.171</v>
+      </c>
+      <c r="K5" t="n">
+        <v>444.325</v>
+      </c>
+      <c r="L5" t="n">
+        <v>444.325</v>
+      </c>
+      <c r="M5" t="n">
+        <v>549.53</v>
+      </c>
+      <c r="N5" t="n">
+        <v>271.419</v>
+      </c>
+      <c r="O5" t="n">
+        <v>224.318</v>
+      </c>
+      <c r="P5" t="n">
+        <v>155.631</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>201.023</v>
+      </c>
+      <c r="R5" t="n">
+        <v>524.985</v>
+      </c>
+      <c r="S5" t="n">
+        <v>659.732</v>
+      </c>
+      <c r="T5" t="n">
+        <v>148.373</v>
+      </c>
+      <c r="U5" t="n">
+        <v>56.473</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>178.826</v>
+      </c>
+      <c r="C6" t="n">
+        <v>178.826</v>
+      </c>
+      <c r="D6" t="n">
+        <v>76.111</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9.33</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>87.544</v>
+      </c>
+      <c r="H6" t="n">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>244.763</v>
+      </c>
+      <c r="J6" t="n">
+        <v>216.373</v>
+      </c>
+      <c r="K6" t="n">
+        <v>450.898</v>
+      </c>
+      <c r="L6" t="n">
+        <v>450.898</v>
+      </c>
+      <c r="M6" t="n">
+        <v>550.732</v>
+      </c>
+      <c r="N6" t="n">
+        <v>264.996</v>
+      </c>
+      <c r="O6" t="n">
+        <v>217.895</v>
+      </c>
+      <c r="P6" t="n">
+        <v>149.208</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>202.225</v>
+      </c>
+      <c r="R6" t="n">
+        <v>526.187</v>
+      </c>
+      <c r="S6" t="n">
+        <v>660.934</v>
+      </c>
+      <c r="T6" t="n">
+        <v>149.575</v>
+      </c>
+      <c r="U6" t="n">
+        <v>57.675</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>248.055</v>
+      </c>
+      <c r="C7" t="n">
+        <v>248.055</v>
+      </c>
+      <c r="D7" t="n">
+        <v>157.847</v>
+      </c>
+      <c r="E7" t="n">
+        <v>79.096</v>
+      </c>
+      <c r="F7" t="n">
+        <v>74.65000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>21.569</v>
+      </c>
+      <c r="I7" t="n">
+        <v>189.826</v>
+      </c>
+      <c r="J7" t="n">
+        <v>161.428</v>
+      </c>
+      <c r="K7" t="n">
+        <v>395.953</v>
+      </c>
+      <c r="L7" t="n">
+        <v>395.953</v>
+      </c>
+      <c r="M7" t="n">
+        <v>495.795</v>
+      </c>
+      <c r="N7" t="n">
+        <v>341.956</v>
+      </c>
+      <c r="O7" t="n">
+        <v>294.855</v>
+      </c>
+      <c r="P7" t="n">
+        <v>230.944</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>147.288</v>
+      </c>
+      <c r="R7" t="n">
+        <v>471.25</v>
+      </c>
+      <c r="S7" t="n">
+        <v>605.997</v>
+      </c>
+      <c r="T7" t="n">
+        <v>94.63800000000001</v>
+      </c>
+      <c r="U7" t="n">
+        <v>23.068</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>239.106</v>
+      </c>
+      <c r="C8" t="n">
+        <v>239.106</v>
+      </c>
+      <c r="D8" t="n">
+        <v>136.391</v>
+      </c>
+      <c r="E8" t="n">
+        <v>70.14700000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>65.70099999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20.593</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>186.727</v>
+      </c>
+      <c r="J8" t="n">
+        <v>158.327</v>
+      </c>
+      <c r="K8" t="n">
+        <v>392.852</v>
+      </c>
+      <c r="L8" t="n">
+        <v>392.852</v>
+      </c>
+      <c r="M8" t="n">
+        <v>492.696</v>
+      </c>
+      <c r="N8" t="n">
+        <v>325.276</v>
+      </c>
+      <c r="O8" t="n">
+        <v>278.175</v>
+      </c>
+      <c r="P8" t="n">
+        <v>209.488</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>144.189</v>
+      </c>
+      <c r="R8" t="n">
+        <v>468.151</v>
+      </c>
+      <c r="S8" t="n">
+        <v>602.898</v>
+      </c>
+      <c r="T8" t="n">
+        <v>91.539</v>
+      </c>
+      <c r="U8" t="n">
+        <v>14.119</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>418.424</v>
+      </c>
+      <c r="C9" t="n">
+        <v>418.424</v>
+      </c>
+      <c r="D9" t="n">
+        <v>315.709</v>
+      </c>
+      <c r="E9" t="n">
+        <v>257.028</v>
+      </c>
+      <c r="F9" t="n">
+        <v>245.019</v>
+      </c>
+      <c r="G9" t="n">
+        <v>189.363</v>
+      </c>
+      <c r="H9" t="n">
+        <v>179.431</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>37.021</v>
+      </c>
+      <c r="K9" t="n">
+        <v>229.21</v>
+      </c>
+      <c r="L9" t="n">
+        <v>229.21</v>
+      </c>
+      <c r="M9" t="n">
+        <v>329.725</v>
+      </c>
+      <c r="N9" t="n">
+        <v>504.594</v>
+      </c>
+      <c r="O9" t="n">
+        <v>457.493</v>
+      </c>
+      <c r="P9" t="n">
+        <v>388.806</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>164.994</v>
+      </c>
+      <c r="R9" t="n">
+        <v>294.643</v>
+      </c>
+      <c r="S9" t="n">
+        <v>439.254</v>
+      </c>
+      <c r="T9" t="n">
+        <v>104.834</v>
+      </c>
+      <c r="U9" t="n">
+        <v>193.437</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>389.8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>389.8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>287.063</v>
+      </c>
+      <c r="E10" t="n">
+        <v>228.382</v>
+      </c>
+      <c r="F10" t="n">
+        <v>216.36</v>
+      </c>
+      <c r="G10" t="n">
+        <v>160.723</v>
+      </c>
+      <c r="H10" t="n">
+        <v>150.777</v>
+      </c>
+      <c r="I10" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>230.167</v>
+      </c>
+      <c r="L10" t="n">
+        <v>230.167</v>
+      </c>
+      <c r="M10" t="n">
+        <v>335.372</v>
+      </c>
+      <c r="N10" t="n">
+        <v>475.984</v>
+      </c>
+      <c r="O10" t="n">
+        <v>428.883</v>
+      </c>
+      <c r="P10" t="n">
+        <v>360.196</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>149.212</v>
+      </c>
+      <c r="R10" t="n">
+        <v>362.141</v>
+      </c>
+      <c r="S10" t="n">
+        <v>445.574</v>
+      </c>
+      <c r="T10" t="n">
+        <v>72.002</v>
+      </c>
+      <c r="U10" t="n">
+        <v>164.827</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>618.119</v>
+      </c>
+      <c r="C11" t="n">
+        <v>618.119</v>
+      </c>
+      <c r="D11" t="n">
+        <v>515.3819999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>456.701</v>
+      </c>
+      <c r="F11" t="n">
+        <v>444.679</v>
+      </c>
+      <c r="G11" t="n">
+        <v>389.042</v>
+      </c>
+      <c r="H11" t="n">
+        <v>379.882</v>
+      </c>
+      <c r="I11" t="n">
+        <v>222.903</v>
+      </c>
+      <c r="J11" t="n">
+        <v>230.214</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>110.232</v>
+      </c>
+      <c r="N11" t="n">
+        <v>704.303</v>
+      </c>
+      <c r="O11" t="n">
+        <v>657.202</v>
+      </c>
+      <c r="P11" t="n">
+        <v>588.515</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>377.531</v>
+      </c>
+      <c r="R11" t="n">
+        <v>137.001</v>
+      </c>
+      <c r="S11" t="n">
+        <v>220.434</v>
+      </c>
+      <c r="T11" t="n">
+        <v>300.321</v>
+      </c>
+      <c r="U11" t="n">
+        <v>393.888</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>618.119</v>
+      </c>
+      <c r="C12" t="n">
+        <v>618.119</v>
+      </c>
+      <c r="D12" t="n">
+        <v>515.3819999999999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>456.701</v>
+      </c>
+      <c r="F12" t="n">
+        <v>444.679</v>
+      </c>
+      <c r="G12" t="n">
+        <v>389.042</v>
+      </c>
+      <c r="H12" t="n">
+        <v>379.882</v>
+      </c>
+      <c r="I12" t="n">
+        <v>222.903</v>
+      </c>
+      <c r="J12" t="n">
+        <v>230.214</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>110.232</v>
+      </c>
+      <c r="N12" t="n">
+        <v>704.303</v>
+      </c>
+      <c r="O12" t="n">
+        <v>657.202</v>
+      </c>
+      <c r="P12" t="n">
+        <v>588.515</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>377.531</v>
+      </c>
+      <c r="R12" t="n">
+        <v>137.001</v>
+      </c>
+      <c r="S12" t="n">
+        <v>220.434</v>
+      </c>
+      <c r="T12" t="n">
+        <v>300.321</v>
+      </c>
+      <c r="U12" t="n">
+        <v>393.888</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>724.9930000000001</v>
+      </c>
+      <c r="C13" t="n">
+        <v>724.9930000000001</v>
+      </c>
+      <c r="D13" t="n">
+        <v>622.285</v>
+      </c>
+      <c r="E13" t="n">
+        <v>563.597</v>
+      </c>
+      <c r="F13" t="n">
+        <v>551.582</v>
+      </c>
+      <c r="G13" t="n">
+        <v>495.932</v>
+      </c>
+      <c r="H13" t="n">
+        <v>486</v>
+      </c>
+      <c r="I13" t="n">
+        <v>329.806</v>
+      </c>
+      <c r="J13" t="n">
+        <v>336.332</v>
+      </c>
+      <c r="K13" t="n">
+        <v>111.216</v>
+      </c>
+      <c r="L13" t="n">
+        <v>111.216</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>811.206</v>
+      </c>
+      <c r="O13" t="n">
+        <v>764.105</v>
+      </c>
+      <c r="P13" t="n">
+        <v>695.418</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>484.434</v>
+      </c>
+      <c r="R13" t="n">
+        <v>106.396</v>
+      </c>
+      <c r="S13" t="n">
+        <v>114.497</v>
+      </c>
+      <c r="T13" t="n">
+        <v>407.224</v>
+      </c>
+      <c r="U13" t="n">
+        <v>500.006</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>89.598</v>
+      </c>
+      <c r="C14" t="n">
+        <v>89.598</v>
+      </c>
+      <c r="D14" t="n">
+        <v>232.827</v>
+      </c>
+      <c r="E14" t="n">
+        <v>257.651</v>
+      </c>
+      <c r="F14" t="n">
+        <v>261.421</v>
+      </c>
+      <c r="G14" t="n">
+        <v>338.877</v>
+      </c>
+      <c r="H14" t="n">
+        <v>342.878</v>
+      </c>
+      <c r="I14" t="n">
+        <v>501.041</v>
+      </c>
+      <c r="J14" t="n">
+        <v>472.643</v>
+      </c>
+      <c r="K14" t="n">
+        <v>707.168</v>
+      </c>
+      <c r="L14" t="n">
+        <v>707.168</v>
+      </c>
+      <c r="M14" t="n">
+        <v>807.683</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>47.089</v>
+      </c>
+      <c r="P14" t="n">
+        <v>134.557</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>471.552</v>
+      </c>
+      <c r="R14" t="n">
+        <v>795.514</v>
+      </c>
+      <c r="S14" t="n">
+        <v>930.261</v>
+      </c>
+      <c r="T14" t="n">
+        <v>405.848</v>
+      </c>
+      <c r="U14" t="n">
+        <v>313.953</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>46.538</v>
+      </c>
+      <c r="C15" t="n">
+        <v>46.538</v>
+      </c>
+      <c r="D15" t="n">
+        <v>189.767</v>
+      </c>
+      <c r="E15" t="n">
+        <v>214.591</v>
+      </c>
+      <c r="F15" t="n">
+        <v>218.361</v>
+      </c>
+      <c r="G15" t="n">
+        <v>295.817</v>
+      </c>
+      <c r="H15" t="n">
+        <v>299.818</v>
+      </c>
+      <c r="I15" t="n">
+        <v>457.981</v>
+      </c>
+      <c r="J15" t="n">
+        <v>429.583</v>
+      </c>
+      <c r="K15" t="n">
+        <v>664.1079999999999</v>
+      </c>
+      <c r="L15" t="n">
+        <v>664.1079999999999</v>
+      </c>
+      <c r="M15" t="n">
+        <v>764.623</v>
+      </c>
+      <c r="N15" t="n">
+        <v>49.967</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>123.336</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>415.443</v>
+      </c>
+      <c r="R15" t="n">
+        <v>739.405</v>
+      </c>
+      <c r="S15" t="n">
+        <v>874.152</v>
+      </c>
+      <c r="T15" t="n">
+        <v>362.788</v>
+      </c>
+      <c r="U15" t="n">
+        <v>270.893</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>110.44</v>
+      </c>
+      <c r="C16" t="n">
+        <v>110.44</v>
+      </c>
+      <c r="D16" t="n">
+        <v>125.648</v>
+      </c>
+      <c r="E16" t="n">
+        <v>144.422</v>
+      </c>
+      <c r="F16" t="n">
+        <v>148.192</v>
+      </c>
+      <c r="G16" t="n">
+        <v>230.593</v>
+      </c>
+      <c r="H16" t="n">
+        <v>229.649</v>
+      </c>
+      <c r="I16" t="n">
+        <v>387.812</v>
+      </c>
+      <c r="J16" t="n">
+        <v>359.414</v>
+      </c>
+      <c r="K16" t="n">
+        <v>593.939</v>
+      </c>
+      <c r="L16" t="n">
+        <v>593.939</v>
+      </c>
+      <c r="M16" t="n">
+        <v>694.454</v>
+      </c>
+      <c r="N16" t="n">
+        <v>135.108</v>
+      </c>
+      <c r="O16" t="n">
+        <v>127.838</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>345.274</v>
+      </c>
+      <c r="R16" t="n">
+        <v>669.236</v>
+      </c>
+      <c r="S16" t="n">
+        <v>803.9829999999999</v>
+      </c>
+      <c r="T16" t="n">
+        <v>292.619</v>
+      </c>
+      <c r="U16" t="n">
+        <v>200.724</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>376.058</v>
+      </c>
+      <c r="C17" t="n">
+        <v>376.058</v>
+      </c>
+      <c r="D17" t="n">
+        <v>273.343</v>
+      </c>
+      <c r="E17" t="n">
+        <v>214.662</v>
+      </c>
+      <c r="F17" t="n">
+        <v>202.653</v>
+      </c>
+      <c r="G17" t="n">
+        <v>146.997</v>
+      </c>
+      <c r="H17" t="n">
+        <v>137.065</v>
+      </c>
+      <c r="I17" t="n">
+        <v>166.387</v>
+      </c>
+      <c r="J17" t="n">
+        <v>155.143</v>
+      </c>
+      <c r="K17" t="n">
+        <v>389.668</v>
+      </c>
+      <c r="L17" t="n">
+        <v>389.668</v>
+      </c>
+      <c r="M17" t="n">
+        <v>490.107</v>
+      </c>
+      <c r="N17" t="n">
+        <v>473.855</v>
+      </c>
+      <c r="O17" t="n">
+        <v>415.127</v>
+      </c>
+      <c r="P17" t="n">
+        <v>346.44</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>451.145</v>
+      </c>
+      <c r="S17" t="n">
+        <v>599.712</v>
+      </c>
+      <c r="T17" t="n">
+        <v>86.146</v>
+      </c>
+      <c r="U17" t="n">
+        <v>151.071</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>712.6559999999999</v>
+      </c>
+      <c r="C18" t="n">
+        <v>712.6559999999999</v>
+      </c>
+      <c r="D18" t="n">
+        <v>609.941</v>
+      </c>
+      <c r="E18" t="n">
+        <v>558.353</v>
+      </c>
+      <c r="F18" t="n">
+        <v>539.26</v>
+      </c>
+      <c r="G18" t="n">
+        <v>483.595</v>
+      </c>
+      <c r="H18" t="n">
+        <v>473.663</v>
+      </c>
+      <c r="I18" t="n">
+        <v>295.317</v>
+      </c>
+      <c r="J18" t="n">
+        <v>324.012</v>
+      </c>
+      <c r="K18" t="n">
+        <v>137.478</v>
+      </c>
+      <c r="L18" t="n">
+        <v>137.478</v>
+      </c>
+      <c r="M18" t="n">
+        <v>101.3</v>
+      </c>
+      <c r="N18" t="n">
+        <v>797.443</v>
+      </c>
+      <c r="O18" t="n">
+        <v>751.725</v>
+      </c>
+      <c r="P18" t="n">
+        <v>683.038</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>449.882</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>190.437</v>
+      </c>
+      <c r="T18" t="n">
+        <v>394.904</v>
+      </c>
+      <c r="U18" t="n">
+        <v>487.669</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>833.633</v>
+      </c>
+      <c r="C19" t="n">
+        <v>833.633</v>
+      </c>
+      <c r="D19" t="n">
+        <v>730.925</v>
+      </c>
+      <c r="E19" t="n">
+        <v>672.244</v>
+      </c>
+      <c r="F19" t="n">
+        <v>660.222</v>
+      </c>
+      <c r="G19" t="n">
+        <v>604.572</v>
+      </c>
+      <c r="H19" t="n">
+        <v>594.64</v>
+      </c>
+      <c r="I19" t="n">
+        <v>438.446</v>
+      </c>
+      <c r="J19" t="n">
+        <v>444.972</v>
+      </c>
+      <c r="K19" t="n">
+        <v>219.856</v>
+      </c>
+      <c r="L19" t="n">
+        <v>219.856</v>
+      </c>
+      <c r="M19" t="n">
+        <v>114.08</v>
+      </c>
+      <c r="N19" t="n">
+        <v>919.846</v>
+      </c>
+      <c r="O19" t="n">
+        <v>872.745</v>
+      </c>
+      <c r="P19" t="n">
+        <v>804.058</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>597.932</v>
+      </c>
+      <c r="R19" t="n">
+        <v>195.178</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>515.864</v>
+      </c>
+      <c r="U19" t="n">
+        <v>608.646</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>321.066</v>
+      </c>
+      <c r="C20" t="n">
+        <v>321.066</v>
+      </c>
+      <c r="D20" t="n">
+        <v>218.38</v>
+      </c>
+      <c r="E20" t="n">
+        <v>152.136</v>
+      </c>
+      <c r="F20" t="n">
+        <v>147.661</v>
+      </c>
+      <c r="G20" t="n">
+        <v>91.992</v>
+      </c>
+      <c r="H20" t="n">
+        <v>82.07299999999999</v>
+      </c>
+      <c r="I20" t="n">
+        <v>103.92</v>
+      </c>
+      <c r="J20" t="n">
+        <v>73.123</v>
+      </c>
+      <c r="K20" t="n">
+        <v>307.648</v>
+      </c>
+      <c r="L20" t="n">
+        <v>307.648</v>
+      </c>
+      <c r="M20" t="n">
+        <v>407.498</v>
+      </c>
+      <c r="N20" t="n">
+        <v>407.266</v>
+      </c>
+      <c r="O20" t="n">
+        <v>360.165</v>
+      </c>
+      <c r="P20" t="n">
+        <v>291.478</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>83.202</v>
+      </c>
+      <c r="R20" t="n">
+        <v>395.803</v>
+      </c>
+      <c r="S20" t="n">
+        <v>517.7</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>96.07899999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>232.246</v>
+      </c>
+      <c r="C21" t="n">
+        <v>232.246</v>
+      </c>
+      <c r="D21" t="n">
+        <v>129.531</v>
+      </c>
+      <c r="E21" t="n">
+        <v>63.287</v>
+      </c>
+      <c r="F21" t="n">
+        <v>58.841</v>
+      </c>
+      <c r="G21" t="n">
+        <v>28.254</v>
+      </c>
+      <c r="H21" t="n">
+        <v>35.877</v>
+      </c>
+      <c r="I21" t="n">
+        <v>194.04</v>
+      </c>
+      <c r="J21" t="n">
+        <v>165.642</v>
+      </c>
+      <c r="K21" t="n">
+        <v>400.167</v>
+      </c>
+      <c r="L21" t="n">
+        <v>400.167</v>
+      </c>
+      <c r="M21" t="n">
+        <v>500.682</v>
+      </c>
+      <c r="N21" t="n">
+        <v>318.416</v>
+      </c>
+      <c r="O21" t="n">
+        <v>271.315</v>
+      </c>
+      <c r="P21" t="n">
+        <v>202.628</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>151.502</v>
+      </c>
+      <c r="R21" t="n">
+        <v>475.464</v>
+      </c>
+      <c r="S21" t="n">
+        <v>610.211</v>
+      </c>
+      <c r="T21" t="n">
+        <v>98.852</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="U1" s="7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5610</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6754</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6852</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9982</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9920</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15577</v>
+      </c>
+      <c r="J2" t="n">
+        <v>14839</v>
+      </c>
+      <c r="K2" t="n">
+        <v>23766</v>
+      </c>
+      <c r="L2" t="n">
+        <v>23766</v>
+      </c>
+      <c r="M2" t="n">
+        <v>27121</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4355</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1980</v>
+      </c>
+      <c r="P2" t="n">
+        <v>6001</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>13855</v>
+      </c>
+      <c r="R2" t="n">
+        <v>28148</v>
+      </c>
+      <c r="S2" t="n">
+        <v>31319</v>
+      </c>
+      <c r="T2" t="n">
+        <v>12563</v>
+      </c>
+      <c r="U2" t="n">
+        <v>8822</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5610</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6754</v>
+      </c>
+      <c r="F3" t="n">
+        <v>6852</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9973</v>
+      </c>
+      <c r="H3" t="n">
+        <v>9911</v>
+      </c>
+      <c r="I3" t="n">
+        <v>15577</v>
+      </c>
+      <c r="J3" t="n">
+        <v>14839</v>
+      </c>
+      <c r="K3" t="n">
+        <v>23757</v>
+      </c>
+      <c r="L3" t="n">
+        <v>23757</v>
+      </c>
+      <c r="M3" t="n">
+        <v>27122</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4355</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1980</v>
+      </c>
+      <c r="P3" t="n">
+        <v>5992</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>13845</v>
+      </c>
+      <c r="R3" t="n">
+        <v>28139</v>
+      </c>
+      <c r="S3" t="n">
+        <v>31310</v>
+      </c>
+      <c r="T3" t="n">
+        <v>12553</v>
+      </c>
+      <c r="U3" t="n">
+        <v>8813</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5818</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5818</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3085</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3156</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6618</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6558</v>
+      </c>
+      <c r="I4" t="n">
+        <v>12213</v>
+      </c>
+      <c r="J4" t="n">
+        <v>11329</v>
+      </c>
+      <c r="K4" t="n">
+        <v>20248</v>
+      </c>
+      <c r="L4" t="n">
+        <v>20248</v>
+      </c>
+      <c r="M4" t="n">
+        <v>23716</v>
+      </c>
+      <c r="N4" t="n">
+        <v>9892</v>
+      </c>
+      <c r="O4" t="n">
+        <v>7486</v>
+      </c>
+      <c r="P4" t="n">
+        <v>5322</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>10491</v>
+      </c>
+      <c r="R4" t="n">
+        <v>24832</v>
+      </c>
+      <c r="S4" t="n">
+        <v>27848</v>
+      </c>
+      <c r="T4" t="n">
+        <v>9061</v>
+      </c>
+      <c r="U4" t="n">
+        <v>5450</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>7061</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7061</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3823</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>630</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3273</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3144</v>
+      </c>
+      <c r="I5" t="n">
+        <v>9217</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8204</v>
+      </c>
+      <c r="K5" t="n">
+        <v>16638</v>
+      </c>
+      <c r="L5" t="n">
+        <v>16638</v>
+      </c>
+      <c r="M5" t="n">
+        <v>20473</v>
+      </c>
+      <c r="N5" t="n">
+        <v>10773</v>
+      </c>
+      <c r="O5" t="n">
+        <v>8366</v>
+      </c>
+      <c r="P5" t="n">
+        <v>5924</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>7495</v>
+      </c>
+      <c r="R5" t="n">
+        <v>21877</v>
+      </c>
+      <c r="S5" t="n">
+        <v>24862</v>
+      </c>
+      <c r="T5" t="n">
+        <v>5962</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6755</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6755</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3145</v>
+      </c>
+      <c r="E6" t="n">
+        <v>701</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3792</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3651</v>
+      </c>
+      <c r="I6" t="n">
+        <v>9297</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8289</v>
+      </c>
+      <c r="K6" t="n">
+        <v>17208</v>
+      </c>
+      <c r="L6" t="n">
+        <v>17208</v>
+      </c>
+      <c r="M6" t="n">
+        <v>20557</v>
+      </c>
+      <c r="N6" t="n">
+        <v>10466</v>
+      </c>
+      <c r="O6" t="n">
+        <v>8059</v>
+      </c>
+      <c r="P6" t="n">
+        <v>5618</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>7575</v>
+      </c>
+      <c r="R6" t="n">
+        <v>21956</v>
+      </c>
+      <c r="S6" t="n">
+        <v>24942</v>
+      </c>
+      <c r="T6" t="n">
+        <v>6046</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9474</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9474</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6651</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3104</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2853</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1223</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7507</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6370</v>
+      </c>
+      <c r="K7" t="n">
+        <v>15290</v>
+      </c>
+      <c r="L7" t="n">
+        <v>15290</v>
+      </c>
+      <c r="M7" t="n">
+        <v>18644</v>
+      </c>
+      <c r="N7" t="n">
+        <v>13539</v>
+      </c>
+      <c r="O7" t="n">
+        <v>11129</v>
+      </c>
+      <c r="P7" t="n">
+        <v>8741</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>5780</v>
+      </c>
+      <c r="R7" t="n">
+        <v>20187</v>
+      </c>
+      <c r="S7" t="n">
+        <v>23169</v>
+      </c>
+      <c r="T7" t="n">
+        <v>4160</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8914</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8914</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5685</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2687</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2428</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1244</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7296</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6149</v>
+      </c>
+      <c r="K8" t="n">
+        <v>15067</v>
+      </c>
+      <c r="L8" t="n">
+        <v>15067</v>
+      </c>
+      <c r="M8" t="n">
+        <v>18421</v>
+      </c>
+      <c r="N8" t="n">
+        <v>12626</v>
+      </c>
+      <c r="O8" t="n">
+        <v>10218</v>
+      </c>
+      <c r="P8" t="n">
+        <v>7776</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>5569</v>
+      </c>
+      <c r="R8" t="n">
+        <v>19976</v>
+      </c>
+      <c r="S8" t="n">
+        <v>22968</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3941</v>
+      </c>
+      <c r="U8" t="n">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15512</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15512</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12285</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9854</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9327</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7444</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6966</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1606</v>
+      </c>
+      <c r="K9" t="n">
+        <v>9200</v>
+      </c>
+      <c r="L9" t="n">
+        <v>9200</v>
+      </c>
+      <c r="M9" t="n">
+        <v>12668</v>
+      </c>
+      <c r="N9" t="n">
+        <v>19249</v>
+      </c>
+      <c r="O9" t="n">
+        <v>16816</v>
+      </c>
+      <c r="P9" t="n">
+        <v>14375</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>6875</v>
+      </c>
+      <c r="R9" t="n">
+        <v>13877</v>
+      </c>
+      <c r="S9" t="n">
+        <v>17307</v>
+      </c>
+      <c r="T9" t="n">
+        <v>4380</v>
+      </c>
+      <c r="U9" t="n">
+        <v>7316</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>14386</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14386</v>
+      </c>
+      <c r="D10" t="n">
+        <v>11105</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8678</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8154</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6305</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5790</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1623</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>8696</v>
+      </c>
+      <c r="L10" t="n">
+        <v>8696</v>
+      </c>
+      <c r="M10" t="n">
+        <v>12530</v>
+      </c>
+      <c r="N10" t="n">
+        <v>18134</v>
+      </c>
+      <c r="O10" t="n">
+        <v>15704</v>
+      </c>
+      <c r="P10" t="n">
+        <v>13264</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>6167</v>
+      </c>
+      <c r="R10" t="n">
+        <v>13503</v>
+      </c>
+      <c r="S10" t="n">
+        <v>17283</v>
+      </c>
+      <c r="T10" t="n">
+        <v>2866</v>
+      </c>
+      <c r="U10" t="n">
+        <v>6190</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>23595</v>
+      </c>
+      <c r="C11" t="n">
+        <v>23595</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20212</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17755</v>
+      </c>
+      <c r="F11" t="n">
+        <v>17231</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15475</v>
+      </c>
+      <c r="H11" t="n">
+        <v>14762</v>
+      </c>
+      <c r="I11" t="n">
+        <v>8722</v>
+      </c>
+      <c r="J11" t="n">
+        <v>8650</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>4623</v>
+      </c>
+      <c r="N11" t="n">
+        <v>27306</v>
+      </c>
+      <c r="O11" t="n">
+        <v>24906</v>
+      </c>
+      <c r="P11" t="n">
+        <v>22466</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>14937</v>
+      </c>
+      <c r="R11" t="n">
+        <v>5597</v>
+      </c>
+      <c r="S11" t="n">
+        <v>8975</v>
+      </c>
+      <c r="T11" t="n">
+        <v>11899</v>
+      </c>
+      <c r="U11" t="n">
+        <v>15116</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>23595</v>
+      </c>
+      <c r="C12" t="n">
+        <v>23595</v>
+      </c>
+      <c r="D12" t="n">
+        <v>20212</v>
+      </c>
+      <c r="E12" t="n">
+        <v>17755</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17231</v>
+      </c>
+      <c r="G12" t="n">
+        <v>15475</v>
+      </c>
+      <c r="H12" t="n">
+        <v>14762</v>
+      </c>
+      <c r="I12" t="n">
+        <v>8722</v>
+      </c>
+      <c r="J12" t="n">
+        <v>8650</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4623</v>
+      </c>
+      <c r="N12" t="n">
+        <v>27306</v>
+      </c>
+      <c r="O12" t="n">
+        <v>24906</v>
+      </c>
+      <c r="P12" t="n">
+        <v>22466</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>14937</v>
+      </c>
+      <c r="R12" t="n">
+        <v>5597</v>
+      </c>
+      <c r="S12" t="n">
+        <v>8975</v>
+      </c>
+      <c r="T12" t="n">
+        <v>11899</v>
+      </c>
+      <c r="U12" t="n">
+        <v>15116</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>27308</v>
+      </c>
+      <c r="C13" t="n">
+        <v>27308</v>
+      </c>
+      <c r="D13" t="n">
+        <v>24065</v>
+      </c>
+      <c r="E13" t="n">
+        <v>21646</v>
+      </c>
+      <c r="F13" t="n">
+        <v>21117</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19223</v>
+      </c>
+      <c r="H13" t="n">
+        <v>18744</v>
+      </c>
+      <c r="I13" t="n">
+        <v>12419</v>
+      </c>
+      <c r="J13" t="n">
+        <v>12440</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4568</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4568</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>31154</v>
+      </c>
+      <c r="O13" t="n">
+        <v>28767</v>
+      </c>
+      <c r="P13" t="n">
+        <v>26325</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>18792</v>
+      </c>
+      <c r="R13" t="n">
+        <v>4925</v>
+      </c>
+      <c r="S13" t="n">
+        <v>5043</v>
+      </c>
+      <c r="T13" t="n">
+        <v>15764</v>
+      </c>
+      <c r="U13" t="n">
+        <v>19108</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4062</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4062</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9551</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10088</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10186</v>
+      </c>
+      <c r="G14" t="n">
+        <v>13260</v>
+      </c>
+      <c r="H14" t="n">
+        <v>13254</v>
+      </c>
+      <c r="I14" t="n">
+        <v>18912</v>
+      </c>
+      <c r="J14" t="n">
+        <v>18288</v>
+      </c>
+      <c r="K14" t="n">
+        <v>27204</v>
+      </c>
+      <c r="L14" t="n">
+        <v>27204</v>
+      </c>
+      <c r="M14" t="n">
+        <v>30674</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2277</v>
+      </c>
+      <c r="P14" t="n">
+        <v>5576</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>17094</v>
+      </c>
+      <c r="R14" t="n">
+        <v>31356</v>
+      </c>
+      <c r="S14" t="n">
+        <v>34633</v>
+      </c>
+      <c r="T14" t="n">
+        <v>16008</v>
+      </c>
+      <c r="U14" t="n">
+        <v>12151</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7689</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8226</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8324</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11398</v>
+      </c>
+      <c r="H15" t="n">
+        <v>11392</v>
+      </c>
+      <c r="I15" t="n">
+        <v>17049</v>
+      </c>
+      <c r="J15" t="n">
+        <v>16379</v>
+      </c>
+      <c r="K15" t="n">
+        <v>25296</v>
+      </c>
+      <c r="L15" t="n">
+        <v>25296</v>
+      </c>
+      <c r="M15" t="n">
+        <v>28766</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2673</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>6369</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>15322</v>
+      </c>
+      <c r="R15" t="n">
+        <v>29602</v>
+      </c>
+      <c r="S15" t="n">
+        <v>32826</v>
+      </c>
+      <c r="T15" t="n">
+        <v>14105</v>
+      </c>
+      <c r="U15" t="n">
+        <v>10292</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5982</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5982</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5420</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5632</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5730</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8860</v>
+      </c>
+      <c r="H16" t="n">
+        <v>8800</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14455</v>
+      </c>
+      <c r="J16" t="n">
+        <v>13680</v>
+      </c>
+      <c r="K16" t="n">
+        <v>22598</v>
+      </c>
+      <c r="L16" t="n">
+        <v>22598</v>
+      </c>
+      <c r="M16" t="n">
+        <v>26067</v>
+      </c>
+      <c r="N16" t="n">
+        <v>6106</v>
+      </c>
+      <c r="O16" t="n">
+        <v>6470</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>12733</v>
+      </c>
+      <c r="R16" t="n">
+        <v>27040</v>
+      </c>
+      <c r="S16" t="n">
+        <v>30160</v>
+      </c>
+      <c r="T16" t="n">
+        <v>11437</v>
+      </c>
+      <c r="U16" t="n">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>13970</v>
+      </c>
+      <c r="C17" t="n">
+        <v>13970</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10742</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8317</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7790</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5906</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5429</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7346</v>
+      </c>
+      <c r="J17" t="n">
+        <v>6005</v>
+      </c>
+      <c r="K17" t="n">
+        <v>14926</v>
+      </c>
+      <c r="L17" t="n">
+        <v>14926</v>
+      </c>
+      <c r="M17" t="n">
+        <v>18270</v>
+      </c>
+      <c r="N17" t="n">
+        <v>17854</v>
+      </c>
+      <c r="O17" t="n">
+        <v>15274</v>
+      </c>
+      <c r="P17" t="n">
+        <v>12834</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>19396</v>
+      </c>
+      <c r="S17" t="n">
+        <v>22831</v>
+      </c>
+      <c r="T17" t="n">
+        <v>3443</v>
+      </c>
+      <c r="U17" t="n">
+        <v>5778</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>29148</v>
+      </c>
+      <c r="C18" t="n">
+        <v>29148</v>
+      </c>
+      <c r="D18" t="n">
+        <v>25899</v>
+      </c>
+      <c r="E18" t="n">
+        <v>23909</v>
+      </c>
+      <c r="F18" t="n">
+        <v>22978</v>
+      </c>
+      <c r="G18" t="n">
+        <v>21075</v>
+      </c>
+      <c r="H18" t="n">
+        <v>20597</v>
+      </c>
+      <c r="I18" t="n">
+        <v>13930</v>
+      </c>
+      <c r="J18" t="n">
+        <v>14290</v>
+      </c>
+      <c r="K18" t="n">
+        <v>5674</v>
+      </c>
+      <c r="L18" t="n">
+        <v>5674</v>
+      </c>
+      <c r="M18" t="n">
+        <v>4534</v>
+      </c>
+      <c r="N18" t="n">
+        <v>31998</v>
+      </c>
+      <c r="O18" t="n">
+        <v>30443</v>
+      </c>
+      <c r="P18" t="n">
+        <v>27998</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>19210</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>7417</v>
+      </c>
+      <c r="T18" t="n">
+        <v>17641</v>
+      </c>
+      <c r="U18" t="n">
+        <v>20956</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>31522</v>
+      </c>
+      <c r="C19" t="n">
+        <v>31522</v>
+      </c>
+      <c r="D19" t="n">
+        <v>28265</v>
+      </c>
+      <c r="E19" t="n">
+        <v>25873</v>
+      </c>
+      <c r="F19" t="n">
+        <v>25344</v>
+      </c>
+      <c r="G19" t="n">
+        <v>23460</v>
+      </c>
+      <c r="H19" t="n">
+        <v>22983</v>
+      </c>
+      <c r="I19" t="n">
+        <v>16698</v>
+      </c>
+      <c r="J19" t="n">
+        <v>16720</v>
+      </c>
+      <c r="K19" t="n">
+        <v>8849</v>
+      </c>
+      <c r="L19" t="n">
+        <v>8849</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4924</v>
+      </c>
+      <c r="N19" t="n">
+        <v>35336</v>
+      </c>
+      <c r="O19" t="n">
+        <v>32972</v>
+      </c>
+      <c r="P19" t="n">
+        <v>30528</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>22473</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7603</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>20068</v>
+      </c>
+      <c r="U19" t="n">
+        <v>23332</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>11910</v>
+      </c>
+      <c r="C20" t="n">
+        <v>11910</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8689</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6010</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5733</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3929</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3189</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4331</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2702</v>
+      </c>
+      <c r="K20" t="n">
+        <v>11844</v>
+      </c>
+      <c r="L20" t="n">
+        <v>11844</v>
+      </c>
+      <c r="M20" t="n">
+        <v>15199</v>
+      </c>
+      <c r="N20" t="n">
+        <v>15654</v>
+      </c>
+      <c r="O20" t="n">
+        <v>13234</v>
+      </c>
+      <c r="P20" t="n">
+        <v>10794</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>3041</v>
+      </c>
+      <c r="R20" t="n">
+        <v>16926</v>
+      </c>
+      <c r="S20" t="n">
+        <v>19963</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>3722</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>8723</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8723</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5492</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2525</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2265</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1550</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1694</v>
+      </c>
+      <c r="I21" t="n">
+        <v>7513</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6376</v>
+      </c>
+      <c r="K21" t="n">
+        <v>15297</v>
+      </c>
+      <c r="L21" t="n">
+        <v>15297</v>
+      </c>
+      <c r="M21" t="n">
+        <v>18765</v>
+      </c>
+      <c r="N21" t="n">
+        <v>12435</v>
+      </c>
+      <c r="O21" t="n">
+        <v>10027</v>
+      </c>
+      <c r="P21" t="n">
+        <v>7585</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>5786</v>
+      </c>
+      <c r="R21" t="n">
+        <v>20192</v>
+      </c>
+      <c r="S21" t="n">
+        <v>23167</v>
+      </c>
+      <c r="T21" t="n">
+        <v>4168</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>